<commit_message>
Creating fields using Excel
</commit_message>
<xml_diff>
--- a/src/Config/AzDevOps-DIT.xlsx
+++ b/src/Config/AzDevOps-DIT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\github-tasb\ado-singleproject-dsc\src\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60B4C7C-9C96-4F4A-9CAC-0D3EB46912A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7F93B0-182B-4414-8D28-ABD121BC5573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33420" yWindow="0" windowWidth="24180" windowHeight="20880" tabRatio="520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8295" windowWidth="29040" windowHeight="15840" tabRatio="520" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Fields Request'!$A$1:$N$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">InitialFields!$A$1:$L$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WitFields!$A$1:$L$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WitFields!$A$1:$L$65</definedName>
     <definedName name="ProjectList">#REF!</definedName>
     <definedName name="TeamsList" localSheetId="6">Table1[Name]</definedName>
     <definedName name="TeamsList">Table1[Name]</definedName>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5190" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5162" uniqueCount="1171">
   <si>
     <t>Name</t>
   </si>
@@ -3754,6 +3754,81 @@
   </si>
   <si>
     <t>Personal Data management</t>
+  </si>
+  <si>
+    <t>0 - Qualitative; 1 - Mandatory; 2 - Benefit; 3 - Stategic</t>
+  </si>
+  <si>
+    <t>Epic; Feature</t>
+  </si>
+  <si>
+    <t>Pressupostos</t>
+  </si>
+  <si>
+    <t>Nome dos campos tem de ser sempre único</t>
+  </si>
+  <si>
+    <t>Campos html não associa com grupo mas sim com secções (Section1, Section2, Section3)</t>
+  </si>
+  <si>
+    <t>Grupos são criados sempre na Section1</t>
+  </si>
+  <si>
+    <t>Grupos podem ser movidos usando Portal Azure DevOps</t>
+  </si>
+  <si>
+    <t>Os campos são criados de forma sequêncial</t>
+  </si>
+  <si>
+    <t>WITs devem exisitir previamente</t>
+  </si>
+  <si>
+    <t>Páginas e grupos podem ser criados pelo automatismo</t>
+  </si>
+  <si>
+    <t>Default value de campos bool é "false"</t>
+  </si>
+  <si>
+    <t>Default value de datetime para a data atual deve ser $currentDateTime</t>
+  </si>
+  <si>
+    <t>Num Resources</t>
+  </si>
+  <si>
+    <t>Carateres inválidos no nome do campo: .,;'`:~\/\*|?"&amp;%$!+=()[]{}&lt;&gt;-#</t>
+  </si>
+  <si>
+    <t>$currentDateTime</t>
+  </si>
+  <si>
+    <t>0 - Not Applicable; 1 - Regulatory; 2 - Legal Imposition; 3 - BCE/BDP Recommendation; 4 - RCI Recommendation; 5 - Internal Audit Recommendation; 6 - External Imposition; 7 - Technological Imposition; 8 - Internal Imposition</t>
+  </si>
+  <si>
+    <t>0 - New; 1 - Active; 2 - Ongoing - On time; 3 - Ongoing - Late; 4 - On-Hold; 5 - Closed; 9 - Removed - To not be implemented;</t>
+  </si>
+  <si>
+    <t>Yes; No; TBD</t>
+  </si>
+  <si>
+    <t>Yes; No</t>
+  </si>
+  <si>
+    <t>Personal Data management 2</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>New Solutions Structural changes</t>
+  </si>
+  <si>
+    <t>New Solutions Structural changes - Comments</t>
+  </si>
+  <si>
+    <t>Section2</t>
+  </si>
+  <si>
+    <t>Section3</t>
   </si>
 </sst>
 </file>
@@ -4202,7 +4277,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4599,6 +4674,9 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4607,7 +4685,25 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5974,82 +6070,82 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:J4" totalsRowShown="0" headerRowDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:J4" totalsRowShown="0" headerRowDxfId="59">
   <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Update" dataDxfId="57"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Organization" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Visibility" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Process" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DefaultTeam" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DefaultTeamDescription" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DefaultTeamAdmin" dataDxfId="49" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DefaultIteration" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Update" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Organization" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Visibility" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Process" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DefaultTeam" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DefaultTeamDescription" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DefaultTeamAdmin" dataDxfId="50" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DefaultIteration" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:K215" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:K215" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A1:K215" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Update" dataDxfId="43"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Project" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Area" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TeamAdmin" dataDxfId="37" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="PublishedWiki" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Iteration" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="StartDate" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="EndDate" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Update" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Project" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Area" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TeamAdmin" dataDxfId="38" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="PublishedWiki" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Iteration" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="StartDate" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="EndDate" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:M324" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:M324" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A1:M324" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Update" dataDxfId="27" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Project" dataDxfId="26" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="User" dataDxfId="25" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Team1" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Team2" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Team3" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Team4" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Team5" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Team6" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Team7" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Team8" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Team9" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Team10" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Update" dataDxfId="28" dataCellStyle="Hyperlink"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Project" dataDxfId="27" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="User" dataDxfId="26" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Team1" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Team2" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Team3" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Team4" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Team5" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Team6" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Team7" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Team8" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Team9" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Team10" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:J312" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:J312" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:J312" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="10">
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Update" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Project" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="TeamOwner" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="OtherContributors" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="OtherReaders" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Wiki" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="ApplySecurity" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="TeamType" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Update" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Project" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="TeamOwner" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="OtherContributors" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="OtherReaders" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Wiki" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="ApplySecurity" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="TeamType" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(D2,Table1[[Name]:[TeamAdmin]],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="TeamOwnerAdmin" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="TeamOwnerAdmin" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(D2,Table1[[Name]:[TeamAdmin]],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6058,7 +6154,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{927A04E4-E65B-4E99-93CE-8E262DC6B159}" name="Table5" displayName="Table5" ref="A1:C12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{927A04E4-E65B-4E99-93CE-8E262DC6B159}" name="Table5" displayName="Table5" ref="A1:C12" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:C12" xr:uid="{927A04E4-E65B-4E99-93CE-8E262DC6B159}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7F1F3A3E-B55F-417B-A005-9F8D115F11BF}" name="Name"/>
@@ -6066,6 +6162,16 @@
     <tableColumn id="3" xr3:uid="{078E2249-3DBE-4CE1-8712-DBA65855A7B0}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}" name="Table6" displayName="Table6" ref="C15:C25" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C15:C25" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DB97B8BD-91A5-4492-97D4-72E71F87B26F}" name="Pressupostos"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -25720,13 +25826,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -25784,7 +25889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" hidden="1" customHeight="1">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" s="121" t="s">
         <v>33</v>
       </c>
@@ -25803,9 +25908,6 @@
       <c r="F2" s="36" t="s">
         <v>943</v>
       </c>
-      <c r="G2" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H2" s="25" t="s">
         <v>32</v>
       </c>
@@ -25822,7 +25924,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1">
+    <row r="3" spans="1:12">
       <c r="A3" s="121" t="s">
         <v>33</v>
       </c>
@@ -25839,9 +25941,6 @@
         <v>945</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G3" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H3" s="25" t="s">
@@ -25879,14 +25978,11 @@
       <c r="F4" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G4" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H4" s="25" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="J4" s="21" t="s">
         <v>1144</v>
@@ -25898,7 +25994,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1">
+    <row r="5" spans="1:12">
       <c r="A5" s="121" t="s">
         <v>33</v>
       </c>
@@ -25917,9 +26013,6 @@
       <c r="F5" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G5" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H5" s="25" t="s">
         <v>32</v>
       </c>
@@ -25936,7 +26029,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="60">
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="121" t="s">
         <v>1053</v>
       </c>
@@ -25953,7 +26046,7 @@
         <v>934</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>1119</v>
+        <v>1146</v>
       </c>
       <c r="G6" s="91" t="s">
         <v>1118</v>
@@ -25962,7 +26055,7 @@
         <v>32</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="J6" s="118" t="s">
         <v>941</v>
@@ -25974,9 +26067,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="135" hidden="1">
-      <c r="A7" s="117" t="s">
-        <v>33</v>
+    <row r="7" spans="1:12" ht="105">
+      <c r="A7" s="121" t="s">
+        <v>1053</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>935</v>
@@ -25991,7 +26084,7 @@
         <v>809</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>1122</v>
+        <v>1161</v>
       </c>
       <c r="G7" s="91" t="s">
         <v>1120</v>
@@ -26012,9 +26105,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" hidden="1">
+    <row r="8" spans="1:12" ht="30">
       <c r="A8" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>935</v>
@@ -26031,9 +26124,6 @@
       <c r="F8" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G8" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H8" s="25" t="s">
         <v>33</v>
       </c>
@@ -26041,7 +26131,7 @@
         <v>1113</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>941</v>
+        <v>1144</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>936</v>
@@ -26050,9 +26140,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" hidden="1">
+    <row r="9" spans="1:12" ht="30">
       <c r="A9" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>935</v>
@@ -26069,9 +26159,6 @@
       <c r="F9" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G9" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H9" s="25" t="s">
         <v>33</v>
       </c>
@@ -26088,9 +26175,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" hidden="1">
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>43</v>
@@ -26105,9 +26192,6 @@
         <v>911</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G10" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H10" s="25" t="s">
@@ -26145,9 +26229,6 @@
       <c r="F11" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G11" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H11" s="25" t="s">
         <v>33</v>
       </c>
@@ -26164,9 +26245,9 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1">
+    <row r="12" spans="1:12">
       <c r="A12" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>44</v>
@@ -26183,9 +26264,6 @@
       <c r="F12" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G12" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H12" s="25" t="s">
         <v>33</v>
       </c>
@@ -26202,9 +26280,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1">
+    <row r="13" spans="1:12">
       <c r="A13" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>928</v>
@@ -26219,9 +26297,6 @@
         <v>913</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G13" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H13" s="25" t="s">
@@ -26259,9 +26334,6 @@
       <c r="F14" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G14" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H14" s="25" t="s">
         <v>32</v>
       </c>
@@ -26278,9 +26350,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1">
+    <row r="15" spans="1:12">
       <c r="A15" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22" t="s">
@@ -26295,9 +26367,6 @@
       <c r="F15" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G15" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H15" s="25" t="s">
         <v>32</v>
       </c>
@@ -26314,9 +26383,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1">
+    <row r="16" spans="1:12">
       <c r="A16" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>929</v>
@@ -26333,9 +26402,6 @@
       <c r="F16" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G16" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H16" s="25" t="s">
         <v>32</v>
       </c>
@@ -26352,7 +26418,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1">
+    <row r="17" spans="1:12">
       <c r="A17" s="121" t="s">
         <v>33</v>
       </c>
@@ -26371,9 +26437,6 @@
       <c r="F17" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G17" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H17" s="25" t="s">
         <v>32</v>
       </c>
@@ -26390,9 +26453,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>930</v>
@@ -26409,9 +26472,6 @@
       <c r="F18" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G18" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H18" s="25" t="s">
         <v>33</v>
       </c>
@@ -26428,9 +26488,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30" hidden="1">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>50</v>
@@ -26447,9 +26507,6 @@
       <c r="F19" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G19" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H19" s="25" t="s">
         <v>33</v>
       </c>
@@ -26466,9 +26523,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="30" hidden="1">
+    <row r="20" spans="1:12" ht="30">
       <c r="A20" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>51</v>
@@ -26485,9 +26542,6 @@
       <c r="F20" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G20" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H20" s="25" t="s">
         <v>33</v>
       </c>
@@ -26504,9 +26558,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="105" hidden="1">
+    <row r="21" spans="1:12" ht="60">
       <c r="A21" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>52</v>
@@ -26521,7 +26575,7 @@
         <v>916</v>
       </c>
       <c r="F21" s="91" t="s">
-        <v>1123</v>
+        <v>1162</v>
       </c>
       <c r="G21" s="91" t="s">
         <v>1121</v>
@@ -26542,9 +26596,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1">
+    <row r="22" spans="1:12">
       <c r="A22" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>53</v>
@@ -26561,9 +26615,6 @@
       <c r="F22" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G22" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H22" s="25" t="s">
         <v>33</v>
       </c>
@@ -26571,7 +26622,7 @@
         <v>938</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>940</v>
+        <v>1169</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>936</v>
@@ -26580,7 +26631,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1">
+    <row r="23" spans="1:12">
       <c r="A23" s="121" t="s">
         <v>33</v>
       </c>
@@ -26598,9 +26649,6 @@
       </c>
       <c r="F23" s="36" t="s">
         <v>943</v>
-      </c>
-      <c r="G23" s="36" t="s">
-        <v>812</v>
       </c>
       <c r="H23" s="25" t="s">
         <v>32</v>
@@ -26637,9 +26685,6 @@
       <c r="F24" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G24" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H24" s="25" t="s">
         <v>33</v>
       </c>
@@ -26656,9 +26701,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>58</v>
@@ -26675,9 +26720,6 @@
       <c r="F25" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G25" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H25" s="25" t="s">
         <v>33</v>
       </c>
@@ -26694,9 +26736,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12">
       <c r="A26" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>59</v>
@@ -26714,13 +26756,13 @@
         <v>812</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>812</v>
+        <v>1160</v>
       </c>
       <c r="H26" s="25" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>938</v>
+        <v>1147</v>
       </c>
       <c r="J26" s="21" t="s">
         <v>940</v>
@@ -26732,9 +26774,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1">
+    <row r="27" spans="1:12">
       <c r="A27" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>60</v>
@@ -26751,9 +26793,6 @@
       <c r="F27" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G27" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H27" s="25" t="s">
         <v>33</v>
       </c>
@@ -26770,9 +26809,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1">
+    <row r="28" spans="1:12">
       <c r="A28" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>61</v>
@@ -26789,9 +26828,6 @@
       <c r="F28" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G28" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H28" s="25" t="s">
         <v>33</v>
       </c>
@@ -26808,9 +26844,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1">
+    <row r="29" spans="1:12">
       <c r="A29" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>63</v>
@@ -26825,9 +26861,6 @@
         <v>65</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G29" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H29" s="25" t="s">
@@ -26865,9 +26898,6 @@
       <c r="F30" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G30" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H30" s="25" t="s">
         <v>33</v>
       </c>
@@ -26884,9 +26914,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1">
+    <row r="31" spans="1:12">
       <c r="A31" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>70</v>
@@ -26903,9 +26933,6 @@
       <c r="F31" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G31" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H31" s="25" t="s">
         <v>33</v>
       </c>
@@ -26922,9 +26949,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1">
+    <row r="32" spans="1:12">
       <c r="A32" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B32" s="32" t="s">
         <v>73</v>
@@ -26941,9 +26968,6 @@
       <c r="F32" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G32" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H32" s="25" t="s">
         <v>33</v>
       </c>
@@ -26960,9 +26984,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1">
+    <row r="33" spans="1:12">
       <c r="A33" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>76</v>
@@ -26979,9 +27003,6 @@
       <c r="F33" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G33" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H33" s="25" t="s">
         <v>33</v>
       </c>
@@ -26998,9 +27019,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1">
+    <row r="34" spans="1:12">
       <c r="A34" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>79</v>
@@ -27017,9 +27038,6 @@
       <c r="F34" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G34" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H34" s="25" t="s">
         <v>33</v>
       </c>
@@ -27036,9 +27054,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1">
+    <row r="35" spans="1:12">
       <c r="A35" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B35" s="33" t="s">
         <v>81</v>
@@ -27055,9 +27073,6 @@
       <c r="F35" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G35" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H35" s="25" t="s">
         <v>33</v>
       </c>
@@ -27074,9 +27089,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1">
+    <row r="36" spans="1:12">
       <c r="A36" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>82</v>
@@ -27093,9 +27108,6 @@
       <c r="F36" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G36" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H36" s="25" t="s">
         <v>33</v>
       </c>
@@ -27103,7 +27115,7 @@
         <v>938</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>1108</v>
+        <v>1169</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>936</v>
@@ -27112,9 +27124,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1">
+    <row r="37" spans="1:12">
       <c r="A37" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>84</v>
@@ -27131,9 +27143,6 @@
       <c r="F37" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G37" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H37" s="25" t="s">
         <v>33</v>
       </c>
@@ -27150,9 +27159,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12">
       <c r="A38" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B38" s="34" t="s">
         <v>85</v>
@@ -27167,9 +27176,6 @@
         <v>864</v>
       </c>
       <c r="F38" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G38" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H38" s="25" t="s">
@@ -27196,10 +27202,10 @@
         <v>86</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>865</v>
+        <v>1158</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E39" s="26" t="s">
         <v>866</v>
@@ -27207,9 +27213,6 @@
       <c r="F39" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G39" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H39" s="25" t="s">
         <v>33</v>
       </c>
@@ -27226,9 +27229,9 @@
         <v>850</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12">
       <c r="A40" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B40" s="35" t="s">
         <v>87</v>
@@ -27245,9 +27248,6 @@
       <c r="F40" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G40" s="36" t="s">
-        <v>812</v>
-      </c>
       <c r="H40" s="25" t="s">
         <v>33</v>
       </c>
@@ -27264,13 +27264,13 @@
         <v>850</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" customHeight="1">
+    <row r="41" spans="1:12" ht="30">
       <c r="A41" s="121" t="s">
         <v>1053</v>
       </c>
       <c r="B41" s="171"/>
       <c r="C41" s="170" t="s">
-        <v>1145</v>
+        <v>1165</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>1128</v>
@@ -27281,14 +27281,14 @@
       <c r="F41" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G41" s="36" t="s">
-        <v>812</v>
+      <c r="G41" s="178" t="s">
+        <v>1166</v>
       </c>
       <c r="H41" s="37" t="s">
         <v>32</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="J41" s="21" t="s">
         <v>1105</v>
@@ -27300,34 +27300,31 @@
         <v>805</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1">
+    <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B42" s="171"/>
       <c r="C42" s="170" t="s">
-        <v>872</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>39</v>
+        <v>1145</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>1128</v>
       </c>
       <c r="E42" s="168" t="s">
-        <v>872</v>
+        <v>1095</v>
       </c>
       <c r="F42" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="G42" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="37" t="s">
         <v>32</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>938</v>
+        <v>1147</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K42" s="21" t="s">
         <v>1104</v>
@@ -27336,34 +27333,31 @@
         <v>805</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="45" hidden="1">
+    <row r="43" spans="1:12">
       <c r="A43" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B43" s="171"/>
       <c r="C43" s="170" t="s">
-        <v>553</v>
+        <v>872</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E43" s="168" t="s">
-        <v>873</v>
-      </c>
-      <c r="F43" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G43" s="169" t="s">
-        <v>1124</v>
+        <v>872</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H43" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>938</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K43" s="21" t="s">
         <v>1104</v>
@@ -27372,25 +27366,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1">
+    <row r="44" spans="1:12" ht="30">
       <c r="A44" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B44" s="171"/>
       <c r="C44" s="170" t="s">
-        <v>1106</v>
+        <v>553</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E44" s="168" t="s">
-        <v>1106</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>812</v>
+        <v>873</v>
+      </c>
+      <c r="F44" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G44" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H44" s="25" t="s">
         <v>33</v>
@@ -27399,7 +27393,7 @@
         <v>938</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K44" s="21" t="s">
         <v>1104</v>
@@ -27408,25 +27402,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="45" hidden="1">
+    <row r="45" spans="1:12">
       <c r="A45" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B45" s="171"/>
       <c r="C45" s="170" t="s">
-        <v>554</v>
+        <v>1106</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E45" s="168" t="s">
-        <v>877</v>
-      </c>
-      <c r="F45" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G45" s="169" t="s">
-        <v>1124</v>
+        <v>1106</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H45" s="25" t="s">
         <v>33</v>
@@ -27435,7 +27426,7 @@
         <v>938</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K45" s="21" t="s">
         <v>1104</v>
@@ -27444,25 +27435,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1">
+    <row r="46" spans="1:12" ht="30">
       <c r="A46" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B46" s="171"/>
       <c r="C46" s="170" t="s">
-        <v>878</v>
+        <v>554</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E46" s="168" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F46" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>812</v>
+        <v>877</v>
+      </c>
+      <c r="F46" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G46" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H46" s="25" t="s">
         <v>33</v>
@@ -27471,7 +27462,7 @@
         <v>938</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K46" s="21" t="s">
         <v>1104</v>
@@ -27480,25 +27471,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="45" hidden="1">
+    <row r="47" spans="1:12">
       <c r="A47" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B47" s="171"/>
       <c r="C47" s="170" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E47" s="168" t="s">
-        <v>880</v>
-      </c>
-      <c r="F47" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G47" s="169" t="s">
-        <v>1124</v>
+        <v>1097</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H47" s="25" t="s">
         <v>33</v>
@@ -27507,7 +27495,7 @@
         <v>938</v>
       </c>
       <c r="J47" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K47" s="21" t="s">
         <v>1104</v>
@@ -27516,25 +27504,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12" ht="30">
       <c r="A48" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B48" s="171"/>
       <c r="C48" s="170" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E48" s="168" t="s">
-        <v>881</v>
-      </c>
-      <c r="F48" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G48" s="36" t="s">
-        <v>812</v>
+        <v>880</v>
+      </c>
+      <c r="F48" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G48" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H48" s="25" t="s">
         <v>33</v>
@@ -27543,7 +27531,7 @@
         <v>938</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K48" s="21" t="s">
         <v>1104</v>
@@ -27552,25 +27540,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="45" hidden="1">
+    <row r="49" spans="1:12">
       <c r="A49" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B49" s="171"/>
       <c r="C49" s="170" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E49" s="168" t="s">
-        <v>883</v>
-      </c>
-      <c r="F49" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G49" s="169" t="s">
-        <v>1124</v>
+        <v>881</v>
+      </c>
+      <c r="F49" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H49" s="25" t="s">
         <v>33</v>
@@ -27579,7 +27564,7 @@
         <v>938</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K49" s="21" t="s">
         <v>1104</v>
@@ -27588,25 +27573,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1">
+    <row r="50" spans="1:12" ht="30">
       <c r="A50" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B50" s="171"/>
       <c r="C50" s="170" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E50" s="168" t="s">
-        <v>884</v>
-      </c>
-      <c r="F50" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G50" s="36" t="s">
-        <v>812</v>
+        <v>883</v>
+      </c>
+      <c r="F50" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G50" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H50" s="25" t="s">
         <v>33</v>
@@ -27615,7 +27600,7 @@
         <v>938</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K50" s="21" t="s">
         <v>1104</v>
@@ -27624,25 +27609,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="45" hidden="1">
+    <row r="51" spans="1:12">
       <c r="A51" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B51" s="171"/>
       <c r="C51" s="170" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E51" s="168" t="s">
-        <v>886</v>
-      </c>
-      <c r="F51" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G51" s="169" t="s">
-        <v>1124</v>
+        <v>884</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H51" s="25" t="s">
         <v>33</v>
@@ -27651,7 +27633,7 @@
         <v>938</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K51" s="21" t="s">
         <v>1104</v>
@@ -27660,25 +27642,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1">
+    <row r="52" spans="1:12" ht="30">
       <c r="A52" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B52" s="171"/>
       <c r="C52" s="170" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E52" s="168" t="s">
-        <v>887</v>
-      </c>
-      <c r="F52" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G52" s="36" t="s">
-        <v>812</v>
+        <v>886</v>
+      </c>
+      <c r="F52" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G52" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H52" s="25" t="s">
         <v>33</v>
@@ -27687,7 +27669,7 @@
         <v>938</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K52" s="21" t="s">
         <v>1104</v>
@@ -27696,25 +27678,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="45" hidden="1">
+    <row r="53" spans="1:12">
       <c r="A53" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B53" s="171"/>
       <c r="C53" s="170" t="s">
-        <v>1098</v>
+        <v>887</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E53" s="168" t="s">
-        <v>889</v>
-      </c>
-      <c r="F53" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G53" s="169" t="s">
-        <v>1124</v>
+        <v>887</v>
+      </c>
+      <c r="F53" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H53" s="25" t="s">
         <v>33</v>
@@ -27723,7 +27702,7 @@
         <v>938</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>1104</v>
@@ -27732,25 +27711,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1">
+    <row r="54" spans="1:12" ht="30">
       <c r="A54" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B54" s="171"/>
       <c r="C54" s="170" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E54" s="168" t="s">
-        <v>890</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G54" s="36" t="s">
-        <v>812</v>
+        <v>889</v>
+      </c>
+      <c r="F54" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G54" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H54" s="25" t="s">
         <v>33</v>
@@ -27759,7 +27738,7 @@
         <v>938</v>
       </c>
       <c r="J54" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K54" s="21" t="s">
         <v>1104</v>
@@ -27768,25 +27747,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="45" hidden="1">
+    <row r="55" spans="1:12">
       <c r="A55" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B55" s="171"/>
       <c r="C55" s="170" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E55" s="168" t="s">
-        <v>892</v>
-      </c>
-      <c r="F55" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G55" s="169" t="s">
-        <v>1124</v>
+        <v>890</v>
+      </c>
+      <c r="F55" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H55" s="25" t="s">
         <v>33</v>
@@ -27795,7 +27771,7 @@
         <v>938</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>1104</v>
@@ -27804,25 +27780,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1">
+    <row r="56" spans="1:12">
       <c r="A56" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B56" s="171"/>
       <c r="C56" s="170" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E56" s="168" t="s">
-        <v>893</v>
-      </c>
-      <c r="F56" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G56" s="36" t="s">
-        <v>812</v>
+        <v>892</v>
+      </c>
+      <c r="F56" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G56" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H56" s="25" t="s">
         <v>33</v>
@@ -27831,7 +27807,7 @@
         <v>938</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K56" s="21" t="s">
         <v>1104</v>
@@ -27840,25 +27816,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="45" hidden="1">
+    <row r="57" spans="1:12">
       <c r="A57" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B57" s="171"/>
       <c r="C57" s="170" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E57" s="168" t="s">
-        <v>895</v>
-      </c>
-      <c r="F57" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G57" s="169" t="s">
-        <v>1124</v>
+        <v>893</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H57" s="25" t="s">
         <v>33</v>
@@ -27867,7 +27840,7 @@
         <v>938</v>
       </c>
       <c r="J57" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K57" s="21" t="s">
         <v>1104</v>
@@ -27876,25 +27849,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1">
+    <row r="58" spans="1:12" ht="30">
       <c r="A58" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B58" s="171"/>
       <c r="C58" s="170" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E58" s="168" t="s">
-        <v>896</v>
-      </c>
-      <c r="F58" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G58" s="36" t="s">
-        <v>812</v>
+        <v>895</v>
+      </c>
+      <c r="F58" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G58" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H58" s="25" t="s">
         <v>33</v>
@@ -27903,7 +27876,7 @@
         <v>938</v>
       </c>
       <c r="J58" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>1104</v>
@@ -27912,25 +27885,22 @@
         <v>805</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="45" hidden="1">
+    <row r="59" spans="1:12">
       <c r="A59" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B59" s="171"/>
       <c r="C59" s="170" t="s">
-        <v>555</v>
+        <v>1103</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E59" s="168" t="s">
-        <v>897</v>
-      </c>
-      <c r="F59" s="169" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G59" s="169" t="s">
-        <v>1124</v>
+        <v>896</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H59" s="25" t="s">
         <v>33</v>
@@ -27939,7 +27909,7 @@
         <v>938</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>1105</v>
+        <v>1144</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>1104</v>
@@ -27948,25 +27918,25 @@
         <v>805</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1">
+    <row r="60" spans="1:12" ht="30">
       <c r="A60" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B60" s="171"/>
       <c r="C60" s="170" t="s">
-        <v>898</v>
+        <v>555</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E60" s="168" t="s">
-        <v>898</v>
-      </c>
-      <c r="F60" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G60" s="36" t="s">
-        <v>812</v>
+        <v>897</v>
+      </c>
+      <c r="F60" s="169" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G60" s="169" t="s">
+        <v>1124</v>
       </c>
       <c r="H60" s="25" t="s">
         <v>33</v>
@@ -27975,7 +27945,7 @@
         <v>938</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>1144</v>
+        <v>1105</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>1104</v>
@@ -27984,67 +27954,62 @@
         <v>805</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="30" hidden="1">
+    <row r="61" spans="1:12">
       <c r="A61" s="121" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B61" s="171"/>
+      <c r="C61" s="170" t="s">
+        <v>898</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="168" t="s">
+        <v>898</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>812</v>
+      </c>
+      <c r="H61" s="25" t="s">
         <v>33</v>
-      </c>
-      <c r="B61" s="64"/>
-      <c r="C61" s="64" t="s">
-        <v>901</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E61" s="168" t="s">
-        <v>1111</v>
-      </c>
-      <c r="F61" s="169" t="s">
-        <v>1112</v>
-      </c>
-      <c r="G61" s="169" t="s">
-        <v>1124</v>
-      </c>
-      <c r="H61" s="25" t="s">
-        <v>32</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>938</v>
       </c>
       <c r="J61" s="21" t="s">
-        <v>941</v>
+        <v>1144</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>936</v>
+        <v>1104</v>
       </c>
       <c r="L61" s="36" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1">
+    <row r="62" spans="1:12" ht="30">
       <c r="A62" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B62" s="64"/>
       <c r="C62" s="64" t="s">
-        <v>904</v>
+        <v>1167</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E62" s="168" t="s">
-        <v>904</v>
-      </c>
-      <c r="F62" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G62" s="36" t="s">
-        <v>812</v>
-      </c>
+        <v>1111</v>
+      </c>
+      <c r="F62" s="169" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G62" s="169"/>
       <c r="H62" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I62" s="21" t="s">
-        <v>938</v>
+        <v>1147</v>
       </c>
       <c r="J62" s="21" t="s">
         <v>941</v>
@@ -28056,34 +28021,31 @@
         <v>805</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="30" hidden="1">
+    <row r="63" spans="1:12">
       <c r="A63" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B63" s="64"/>
       <c r="C63" s="64" t="s">
-        <v>1109</v>
+        <v>1168</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>1125</v>
+        <v>39</v>
       </c>
       <c r="E63" s="168" t="s">
-        <v>906</v>
-      </c>
-      <c r="F63" s="169" t="s">
-        <v>1112</v>
-      </c>
-      <c r="G63" s="169" t="s">
-        <v>1124</v>
+        <v>904</v>
+      </c>
+      <c r="F63" s="36" t="s">
+        <v>812</v>
       </c>
       <c r="H63" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I63" s="21" t="s">
         <v>938</v>
       </c>
       <c r="J63" s="21" t="s">
-        <v>941</v>
+        <v>1170</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>936</v>
@@ -28092,28 +28054,26 @@
         <v>805</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1">
+    <row r="64" spans="1:12">
       <c r="A64" s="121" t="s">
-        <v>33</v>
+        <v>1053</v>
       </c>
       <c r="B64" s="64"/>
       <c r="C64" s="64" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>39</v>
+        <v>1125</v>
       </c>
       <c r="E64" s="168" t="s">
-        <v>1110</v>
-      </c>
-      <c r="F64" s="36" t="s">
-        <v>812</v>
-      </c>
-      <c r="G64" s="36" t="s">
-        <v>812</v>
-      </c>
+        <v>906</v>
+      </c>
+      <c r="F64" s="169" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G64" s="169"/>
       <c r="H64" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I64" s="21" t="s">
         <v>938</v>
@@ -28125,26 +28085,53 @@
         <v>936</v>
       </c>
       <c r="L64" s="36" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="121" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B65" s="64"/>
+      <c r="C65" s="64" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" s="168" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F65" s="36" t="s">
+        <v>812</v>
+      </c>
+      <c r="H65" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>938</v>
+      </c>
+      <c r="J65" s="21" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K65" s="21" t="s">
+        <v>936</v>
+      </c>
+      <c r="L65" s="36" t="s">
         <v>805</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="H37:H38 H30:H35 C28:C29 B28 C30:D34 D37:D38 D35" name="Range1_2_3_2"/>
-    <protectedRange sqref="H39:H40 H42:H64 C35:C40" name="Range1_4_3_3"/>
+    <protectedRange sqref="H39:H40 H43:H65 C35:C40" name="Range1_4_3_3"/>
     <protectedRange sqref="B29:B34" name="Range1_2_3_1_1"/>
     <protectedRange sqref="B35:B40" name="Range1_4_3_2_1"/>
   </protectedRanges>
-  <autoFilter ref="A1:L64" xr:uid="{AFD31169-49D4-4C3C-88C8-C4B156B1A1C2}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="C"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L65" xr:uid="{AFD31169-49D4-4C3C-88C8-C4B156B1A1C2}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D64" xr:uid="{0E995BE7-10D9-476C-8F05-22C3A7C330FA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D65" xr:uid="{0E995BE7-10D9-476C-8F05-22C3A7C330FA}">
       <formula1>WitFields</formula1>
     </dataValidation>
   </dataValidations>
@@ -33291,10 +33278,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12EEF22-A151-484C-AB29-0A04222CEC00}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33440,24 +33427,72 @@
       <c r="B13" s="94"/>
       <c r="C13" s="94"/>
     </row>
+    <row r="15" spans="1:3">
+      <c r="C15" s="95" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" t="s">
+        <v>1157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062D84A708F12404A885A4999D57F6C99" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea1fc7de5685a845414805ecad644c80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d4d6018b-bb5f-44df-a9e9-65296ee76512" xmlns:ns4="944e1ce2-6307-47fb-8cdc-aa406f6e8b8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1174c48ca535c5cf57d596e351a71f7a" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -33697,6 +33732,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -33707,14 +33751,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D95FA6E-FB47-4A4A-BC36-FDBCFF225D5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF3FFE8-FCE4-4AC1-9F90-EEFADE2E6928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33734,6 +33770,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D95FA6E-FB47-4A4A-BC36-FDBCFF225D5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23754B3E-E3F1-458D-BC65-E41A16921420}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Create, Delete and Update finished
</commit_message>
<xml_diff>
--- a/src/Config/AzDevOps-DIT.xlsx
+++ b/src/Config/AzDevOps-DIT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\github-tasb\ado-singleproject-dsc\src\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E710A7D5-6D4E-445F-9871-01CF752C36C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAC8D32-24E3-46AF-90C2-D9D0F895DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8295" windowWidth="29040" windowHeight="15840" tabRatio="520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8295" windowWidth="29040" windowHeight="15840" tabRatio="520" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5165" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5164" uniqueCount="1192">
   <si>
     <t>Name</t>
   </si>
@@ -3771,15 +3771,6 @@
     <t>Campos html não associa com grupo mas sim com secções (Section1, Section2, Section3)</t>
   </si>
   <si>
-    <t>Grupos são criados sempre na Section1</t>
-  </si>
-  <si>
-    <t>Grupos podem ser movidos usando Portal Azure DevOps</t>
-  </si>
-  <si>
-    <t>Os campos são criados de forma sequêncial</t>
-  </si>
-  <si>
     <t>WITs devem exisitir previamente</t>
   </si>
   <si>
@@ -3789,21 +3780,12 @@
     <t>Default value de campos bool é "false"</t>
   </si>
   <si>
-    <t>Default value de datetime para a data atual deve ser $currentDateTime</t>
-  </si>
-  <si>
     <t>Num Resources</t>
   </si>
   <si>
-    <t>Carateres inválidos no nome do campo: .,;'`:~\/\*|?"&amp;%$!+=()[]{}&lt;&gt;-#</t>
-  </si>
-  <si>
     <t>$currentDateTime</t>
   </si>
   <si>
-    <t>0 - Not Applicable; 1 - Regulatory; 2 - Legal Imposition; 3 - BCE/BDP Recommendation; 4 - RCI Recommendation; 5 - Internal Audit Recommendation; 6 - External Imposition; 7 - Technological Imposition; 8 - Internal Imposition</t>
-  </si>
-  <si>
     <t>Yes; No; TBD</t>
   </si>
   <si>
@@ -3825,12 +3807,6 @@
     <t>Section3</t>
   </si>
   <si>
-    <t>Delete remove o field dos Work Items mas não elimina o field to processo. Este deverá ser removido manualmente</t>
-  </si>
-  <si>
-    <t>Update não troca tipo de campo nem a sua posição (Grupo / secção). Este ajuste deverá ser feito manualmente ou realizar um delete seguido de um create</t>
-  </si>
-  <si>
     <t>0 - New; 1 - Active; 2 - Ongoing - On time; 3 - Ongoing - Late; 4 - On-Hold; 5 - Closed; 9 - Removed - To not be implemented</t>
   </si>
   <si>
@@ -3883,6 +3859,50 @@
   </si>
   <si>
     <t>Accuracy Comments</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Minha description</t>
+  </si>
+  <si>
+    <t>Value1; Value2; Value3</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carateres inválidos no nome do campo: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="CaskaydiaCove Nerd Font"/>
+        <family val="3"/>
+      </rPr>
+      <t>.,;'`:~\/\*|?"&amp;%$!+=()[]{}&lt;&gt;-#</t>
+    </r>
+  </si>
+  <si>
+    <t>Grupos são criados sempre na Section1, sendo que podem ser movidos no layout da página usando Portal Azure DevOps</t>
+  </si>
+  <si>
+    <t>Os campos são criados de forma sequêncial dentro da mesma Section</t>
+  </si>
+  <si>
+    <t>Caso pretendam Default value de datetime para a data atual deve ser $currentDateTime</t>
+  </si>
+  <si>
+    <t>Update não altera tipo de campo nem a sua posição (Grupo / secção). Este ajuste deverá ser feito manualmente ou realizar um delete seguido de um create</t>
+  </si>
+  <si>
+    <t>Delete remove o campo dos Work Items mas não elimina o campo do processo. Este deverá ser removido manualmente</t>
   </si>
 </sst>
 </file>
@@ -3894,7 +3914,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4055,6 +4075,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="CaskaydiaCove Nerd Font"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="20">
@@ -4333,7 +4359,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4732,6 +4758,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -6222,8 +6251,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}" name="Table6" displayName="Table6" ref="C15:C28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="C15:C28" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}" name="Table6" displayName="Table6" ref="C15:C27" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C15:C27" xr:uid="{35E5C019-4876-422B-B48F-B3E3AF674767}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DB97B8BD-91A5-4492-97D4-72E71F87B26F}" name="Pressupostos"/>
   </tableColumns>
@@ -25884,10 +25913,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42:A44"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26017,7 +26046,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="121" t="s">
-        <v>33</v>
+        <v>1181</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>38</v>
@@ -26029,13 +26058,13 @@
         <v>39</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>40</v>
+        <v>1182</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>812</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>1147</v>
@@ -26123,9 +26152,9 @@
         <v>805</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="121" t="s">
-        <v>33</v>
+        <v>1181</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>935</v>
@@ -26140,10 +26169,10 @@
         <v>809</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>1161</v>
+        <v>1183</v>
       </c>
       <c r="G7" s="91" t="s">
-        <v>1120</v>
+        <v>1184</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>32</v>
@@ -26268,7 +26297,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="121" t="s">
-        <v>33</v>
+        <v>1181</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>927</v>
@@ -26279,8 +26308,8 @@
       <c r="D11" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="91" t="s">
-        <v>817</v>
+      <c r="E11" s="22" t="s">
+        <v>912</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>812</v>
@@ -26616,13 +26645,13 @@
     </row>
     <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="121" t="s">
-        <v>33</v>
+        <v>1185</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>1125</v>
@@ -26631,7 +26660,7 @@
         <v>916</v>
       </c>
       <c r="F21" s="91" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="G21" s="91" t="s">
         <v>1121</v>
@@ -26678,7 +26707,7 @@
         <v>938</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>936</v>
@@ -26812,7 +26841,7 @@
         <v>812</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="H26" s="25" t="s">
         <v>33</v>
@@ -27147,7 +27176,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="121" t="s">
-        <v>33</v>
+        <v>1185</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>82</v>
@@ -27171,7 +27200,7 @@
         <v>938</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="K36" s="21" t="s">
         <v>936</v>
@@ -27258,7 +27287,7 @@
         <v>86</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>1126</v>
@@ -27287,7 +27316,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="121" t="s">
-        <v>33</v>
+        <v>1185</v>
       </c>
       <c r="B40" s="35" t="s">
         <v>87</v>
@@ -27326,7 +27355,7 @@
       </c>
       <c r="B41" s="171"/>
       <c r="C41" s="170" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>1128</v>
@@ -27338,7 +27367,7 @@
         <v>812</v>
       </c>
       <c r="G41" s="172" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="H41" s="37" t="s">
         <v>32</v>
@@ -27395,7 +27424,7 @@
       </c>
       <c r="B43" s="171"/>
       <c r="C43" s="170" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>39</v>
@@ -27437,7 +27466,7 @@
         <v>873</v>
       </c>
       <c r="F44" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G44" s="169" t="s">
         <v>1124</v>
@@ -27460,11 +27489,11 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B45" s="171"/>
       <c r="C45" s="170" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>39</v>
@@ -27493,7 +27522,7 @@
     </row>
     <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B46" s="171"/>
       <c r="C46" s="170" t="s">
@@ -27506,7 +27535,7 @@
         <v>877</v>
       </c>
       <c r="F46" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G46" s="169" t="s">
         <v>1124</v>
@@ -27529,11 +27558,11 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B47" s="171"/>
       <c r="C47" s="170" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
       <c r="D47" s="24" t="s">
         <v>39</v>
@@ -27562,11 +27591,11 @@
     </row>
     <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B48" s="171"/>
       <c r="C48" s="170" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>1125</v>
@@ -27575,7 +27604,7 @@
         <v>880</v>
       </c>
       <c r="F48" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G48" s="169" t="s">
         <v>1124</v>
@@ -27598,11 +27627,11 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B49" s="171"/>
       <c r="C49" s="170" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>39</v>
@@ -27631,11 +27660,11 @@
     </row>
     <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B50" s="171"/>
       <c r="C50" s="170" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>1125</v>
@@ -27644,7 +27673,7 @@
         <v>883</v>
       </c>
       <c r="F50" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G50" s="169" t="s">
         <v>1124</v>
@@ -27667,11 +27696,11 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B51" s="171"/>
       <c r="C51" s="170" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>39</v>
@@ -27700,11 +27729,11 @@
     </row>
     <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B52" s="171"/>
       <c r="C52" s="170" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
       <c r="D52" s="24" t="s">
         <v>1125</v>
@@ -27713,7 +27742,7 @@
         <v>886</v>
       </c>
       <c r="F52" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G52" s="169" t="s">
         <v>1124</v>
@@ -27736,11 +27765,11 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B53" s="171"/>
       <c r="C53" s="170" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>39</v>
@@ -27769,7 +27798,7 @@
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B54" s="171"/>
       <c r="C54" s="170" t="s">
@@ -27782,7 +27811,7 @@
         <v>889</v>
       </c>
       <c r="F54" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G54" s="169" t="s">
         <v>1124</v>
@@ -27805,11 +27834,11 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B55" s="171"/>
       <c r="C55" s="170" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>39</v>
@@ -27838,7 +27867,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B56" s="171"/>
       <c r="C56" s="170" t="s">
@@ -27851,7 +27880,7 @@
         <v>892</v>
       </c>
       <c r="F56" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G56" s="169" t="s">
         <v>1124</v>
@@ -27874,11 +27903,11 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B57" s="171"/>
       <c r="C57" s="170" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>39</v>
@@ -27907,7 +27936,7 @@
     </row>
     <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B58" s="171"/>
       <c r="C58" s="170" t="s">
@@ -27920,7 +27949,7 @@
         <v>895</v>
       </c>
       <c r="F58" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G58" s="169" t="s">
         <v>1124</v>
@@ -27943,11 +27972,11 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B59" s="171"/>
       <c r="C59" s="170" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>39</v>
@@ -27976,7 +28005,7 @@
     </row>
     <row r="60" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B60" s="171"/>
       <c r="C60" s="170" t="s">
@@ -27989,7 +28018,7 @@
         <v>897</v>
       </c>
       <c r="F60" s="169" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="G60" s="169" t="s">
         <v>1124</v>
@@ -28012,11 +28041,11 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B61" s="171"/>
       <c r="C61" s="170" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>39</v>
@@ -28045,11 +28074,11 @@
     </row>
     <row r="62" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B62" s="64"/>
       <c r="C62" s="64" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>1125</v>
@@ -28058,7 +28087,7 @@
         <v>1111</v>
       </c>
       <c r="F62" s="169" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="G62" s="169"/>
       <c r="H62" s="25" t="s">
@@ -28079,11 +28108,11 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B63" s="64"/>
       <c r="C63" s="64" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
       <c r="D63" s="24" t="s">
         <v>39</v>
@@ -28101,7 +28130,7 @@
         <v>938</v>
       </c>
       <c r="J63" s="21" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>936</v>
@@ -28112,7 +28141,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B64" s="64"/>
       <c r="C64" s="64" t="s">
@@ -28125,7 +28154,7 @@
         <v>906</v>
       </c>
       <c r="F64" s="169" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="G64" s="169"/>
       <c r="H64" s="25" t="s">
@@ -28146,11 +28175,11 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="121" t="s">
-        <v>1053</v>
+        <v>33</v>
       </c>
       <c r="B65" s="64"/>
       <c r="C65" s="64" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>39</v>
@@ -28168,7 +28197,7 @@
         <v>938</v>
       </c>
       <c r="J65" s="21" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="K65" s="21" t="s">
         <v>936</v>
@@ -33334,10 +33363,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12EEF22-A151-484C-AB29-0A04222CEC00}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33489,68 +33518,63 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="179" t="s">
         <v>1149</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>1159</v>
+      <c r="C17" s="179" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="179" t="s">
         <v>1150</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="179" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="179" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="179" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="179" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="179" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>1155</v>
-      </c>
-    </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>1156</v>
+      <c r="C24" s="179" t="s">
+        <v>1189</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>1157</v>
+      <c r="C25" s="179" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>1170</v>
+      <c r="C26" s="179" t="s">
+        <v>1191</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>1172</v>
+      <c r="C27" s="179" t="s">
+        <v>1164</v>
       </c>
     </row>
   </sheetData>
@@ -33564,24 +33588,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062D84A708F12404A885A4999D57F6C99" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea1fc7de5685a845414805ecad644c80">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d4d6018b-bb5f-44df-a9e9-65296ee76512" xmlns:ns4="944e1ce2-6307-47fb-8cdc-aa406f6e8b8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1174c48ca535c5cf57d596e351a71f7a" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -33821,25 +33827,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D95FA6E-FB47-4A4A-BC36-FDBCFF225D5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23754B3E-E3F1-458D-BC65-E41A16921420}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF3FFE8-FCE4-4AC1-9F90-EEFADE2E6928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33859,6 +33865,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23754B3E-E3F1-458D-BC65-E41A16921420}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D95FA6E-FB47-4A4A-BC36-FDBCFF225D5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>